<commit_message>
Updating test for instance flattening bug
</commit_message>
<xml_diff>
--- a/pyxform/tests/example_xls/flat_xlsform_test.xlsx
+++ b/pyxform/tests/example_xls/flat_xlsform_test.xlsx
@@ -907,7 +907,7 @@
   <dimension ref="A1:AMN59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1034,41 +1034,50 @@
     </row>
     <row r="3" spans="1:27" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3"/>
+      <c r="N3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:27" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4"/>
+      <c r="Q4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="16.5" customHeight="1">
@@ -1076,18 +1085,13 @@
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6"/>
-      <c r="N6"/>
-      <c r="Q6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="16.5" customHeight="1">
@@ -1095,36 +1099,32 @@
         <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7"/>
-      <c r="N7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R7" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:27" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8"/>
       <c r="N8"/>
       <c r="Q8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="36.6" customHeight="1">

</xml_diff>